<commit_message>
Rimozione corsi interateneo/nuovi aa 2024-2025
</commit_message>
<xml_diff>
--- a/src/dataset/elenco_2024-2025.xlsx
+++ b/src/dataset/elenco_2024-2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,22 +589,25 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>LINGUA E CULTURA ITALIANA PER STRANIERI</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
+          <t>SCIENZE DELL’EDUCAZIONE E DEI PROCESSI FORMATIVI</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3038</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>L-10 Lettere</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>TELEMATICO INTERATENEO
-SEDE AMM.VA PISA</t>
-        </is>
-      </c>
+          <t>L-19 Scienze dell'educazione e della formazione</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Luana Salvarani</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
@@ -615,22 +618,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SCIENZE DELL’EDUCAZIONE E DEI PROCESSI FORMATIVI</t>
+          <t>COMUNICAZIONE E MEDIA CONTEMPORANEI PER LE INDUSTRIE CREATIVE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3038</t>
+          <t>3051</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>L-19 Scienze dell'educazione e della formazione</t>
+          <t>L-20 Scienze della comunicazione</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Luana Salvarani</t>
+          <t>Sara Martin</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -644,26 +647,30 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>COMUNICAZIONE E MEDIA CONTEMPORANEI PER LE INDUSTRIE CREATIVE</t>
+          <t>INTERPRETE DI LINGUA DEI SEGNI ITALIANA E DI LINGUA DEI SEGNI ITALIANA TATTILE</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3051</t>
+          <t>3066</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>L-20 Scienze della comunicazione</t>
+          <t>L-12 Mediazione Linguistica</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sara Martin</t>
+          <t>Davide Astori</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>5  DI CUI 3 PO/PA</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI</t>
@@ -673,30 +680,26 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INTERPRETE DI LINGUA DEI SEGNI ITALIANA E DI LINGUA DEI SEGNI ITALIANA TATTILE</t>
+          <t>LETTERE CLASSICHE E MODERNE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3066</t>
+          <t>5049</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>L-12 Mediazione Linguistica</t>
+          <t>LM-14 Filologia moderna &amp; LM-15 Filologia, letterature e storia dell'antichità</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Davide Astori</t>
+          <t>Gualtiero Rota</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>5  DI CUI 3 PO/PA</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI</t>
@@ -706,22 +709,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LETTERE CLASSICHE E MODERNE</t>
+          <t>GIORNALISMO, CULTURA EDITORIALE, COMUNICAZIONE AMBIENTALE E MULTIMEDIALE</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5049</t>
+          <t>5078</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LM-14 Filologia moderna &amp; LM-15 Filologia, letterature e storia dell'antichità</t>
+          <t>LM-19 Informazione e sistemi editoriali</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Gualtiero Rota</t>
+          <t>Marco Deriu</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -735,22 +738,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GIORNALISMO, CULTURA EDITORIALE, COMUNICAZIONE AMBIENTALE E MULTIMEDIALE</t>
+          <t>PROGETTAZIONE E COORDINAMENTO DEI SERVIZI EDUCATIVI</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5078</t>
+          <t>5046</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LM-19 Informazione e sistemi editoriali</t>
+          <t>LM-50 Programmazione e gestione dei servizi educativi</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Marco Deriu</t>
+          <t>Luana Salvarani</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -764,22 +767,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PROGETTAZIONE E COORDINAMENTO DEI SERVIZI EDUCATIVI</t>
+          <t>PSICOLOGIA DELL’INTERVENTO CLINICO E SOCIALE</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5046</t>
+          <t>5054</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LM-50 Programmazione e gestione dei servizi educativi</t>
+          <t>LM-51 Psicologia</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Luana Salvarani</t>
+          <t>Tiziana Mancini</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -793,22 +796,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PSICOLOGIA DELL’INTERVENTO CLINICO E SOCIALE</t>
+          <t>STORIA E CRITICA DELLE ARTI E DELLO SPETTACOLO</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5054</t>
+          <t>5048</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>LM-51 Psicologia</t>
+          <t>LM-89 Storia dell'arte</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Tiziana Mancini</t>
+          <t>Paolo Russo</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -822,29 +825,25 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>FILOSOFIA</t>
+          <t>LANGUAGE SCIENCES AND CULTURAL STUDIES FOR SPECIAL NEEDS</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5025</t>
+          <t>5073</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LM-78 Scienze filosofiche</t>
+          <t>LM-39 Linguistica</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>HUEMER Wolfgang Andreas</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>CORSO INTERATENEO – SEDE AMM.VA PARMA</t>
-        </is>
-      </c>
+          <t>Michele Daloiso</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
@@ -855,104 +854,108 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>STORIA E CRITICA DELLE ARTI E DELLO SPETTACOLO</t>
+          <t>SCIENZE POLITICHE E DELLE RELAZIONI INTERNAZIONALI</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5048</t>
+          <t>3032</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LM-89 Storia dell'arte</t>
+          <t>L-36 Scienze politiche e delle relazioni internazionali</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Paolo Russo</t>
+          <t>Emanuele Castelli</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI</t>
+          <t>DIPARTIMENTODI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>LANGUAGE SCIENCES AND CULTURAL STUDIES FOR SPECIAL NEEDS</t>
+          <t>SERVIZIO SOCIALE</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5073</t>
+          <t>3006</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LM-39 Linguistica</t>
+          <t>L-39 Servizio sociale</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Michele Daloiso</t>
+          <t>Paola Torretta</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>5  DI CUI 3 PO/PA</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI</t>
+          <t>DIPARTIMENTODI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LINGUE, CULTURE, COMUNICAZIONE</t>
+          <t>GIURISPRUDENZA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5051</t>
+          <t>0995</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LM-37 Lingue e letterature moderne europee e americane</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>INTERATENEO CON MODENA E REGGIO EMILIA – SEDE AMM.VA REGGIO EMILIA</t>
-        </is>
-      </c>
+          <t>LMG/01 Classe delle lauree magistrali in giurisprudenza</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Luca Ghidoni</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI  DI DISCIPLINE UMANISTICHE, SOCIALI E DELLE IMPRESE CULTURALI</t>
+          <t>DIPARTIMENTODI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SCIENZE POLITICHE E DELLE RELAZIONI INTERNAZIONALI</t>
+          <t>RELAZIONI INTERNAZIONALI ED EUROPEE</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3032</t>
+          <t>5044</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>L-36 Scienze politiche e delle relazioni internazionali</t>
+          <t>LM-52 Relazioni internazionali</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -971,17 +974,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SERVIZIO SOCIALE</t>
+          <t>PROGRAMMAZIONE E GESTIONE DEI SERVIZI SOCIALI</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3006</t>
+          <t>5010</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>L-39 Servizio sociale</t>
+          <t>LM-87 Servizio sociale e politiche sociali</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -992,7 +995,7 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>5  DI CUI 3 PO/PA</t>
+          <t>4  DI CUI 2 PO/PA</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1004,146 +1007,142 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GIURISPRUDENZA</t>
+          <t>ARCHITETTURA RIGENERAZIONE SOSTENIBILITÀ</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0995</t>
+          <t>3054</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>LMG/01 Classe delle lauree magistrali in giurisprudenza</t>
+          <t>L-17 Scienze dell'architettura</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Luca Ghidoni</t>
+          <t>Andrea Zerbi</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI</t>
+          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>RELAZIONI INTERNAZIONALI ED EUROPEE</t>
+          <t>COSTRUZIONI, INFRASTRUTTURE E TERRITORIO</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5044</t>
+          <t>3056</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LM-52 Relazioni internazionali</t>
+          <t>L-P01 Professioni tecniche per l’edilizia e il territorio</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Emanuele Castelli</t>
+          <t>Andrea Maranzoni</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>4  DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI</t>
+          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PROGRAMMAZIONE E GESTIONE DEI SERVIZI SOCIALI</t>
+          <t>DESIN SOSTENIBILE PER IL SISTEMA ALIMENTARE</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5010</t>
+          <t>3057</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LM-87 Servizio sociale e politiche sociali</t>
+          <t>L-4 Disegno industriale</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Paola Torretta</t>
+          <t>Paolo Marco Tamborrini</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>4  DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI</t>
+          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GLOBAL FOOD LAW: SUSTAINABILITY CHALLENGES AND INNOVATION</t>
+          <t>INGEGNERIA CIVILE E AMBIENTALE</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5081</t>
+          <t>3007</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LM/SC-GIUR R – Scienze Giuridiche</t>
+          <t>L-7 Ingegneria civile e ambientale</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>REFERENTE: Prof.ssa Lucia Scaffardi</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>ATTIVO DALL’A.A. 2024/25</t>
-        </is>
-      </c>
+          <t>Andrea Zanini</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI  DI GIURISPRUDENZA, STUDI POLITICI E INTERNAZIONALI</t>
+          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ARCHITETTURA RIGENERAZIONE SOSTENIBILITÀ</t>
+          <t>INGEGNERIA DELLE TECNOLOGIE INFORMATICHE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3054</t>
+          <t>3061</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>L-17 Scienze dell'architettura</t>
+          <t>L-8 Ingegneria dell'informazione</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Andrea Zerbi</t>
+          <t>Agostino Poggi</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -1157,30 +1156,26 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>COSTRUZIONI, INFRASTRUTTURE E TERRITORIO</t>
+          <t>INGEGNERIA INFORMATICA, ELETTRONICA E DELLE TELECOMUNICAZIONI</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3056</t>
+          <t>3050</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>L-P01 Professioni tecniche per l’edilizia e il territorio</t>
+          <t>L-8 Ingegneria dell'informazione</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Andrea Maranzoni</t>
+          <t>Gianluigi Ferrari</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>4  DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
@@ -1190,22 +1185,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>DESIN SOSTENIBILE PER IL SISTEMA ALIMENTARE</t>
+          <t>ARCHITETTURA E CITTA’ SOSTENIBILI</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3057</t>
+          <t>5066</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>L-4 Disegno industriale</t>
+          <t>LM-4 Architettura e ingegneria edile-architettura</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Paolo Marco Tamborrini</t>
+          <t>Enrico Prandi</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1219,22 +1214,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>INGEGNERIA CIVILE E AMBIENTALE</t>
+          <t>INGEGNERIA CIVILE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3007</t>
+          <t>5011</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>L-7 Ingegneria civile e ambientale</t>
+          <t>LM-23 Ingegneria civile</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Andrea Zanini</t>
+          <t>Francesco Freddi</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1248,22 +1243,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>INGEGNERIA DELLE TECNOLOGIE INFORMATICHE</t>
+          <t>COMMUNICATION ENGENEERING</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3061</t>
+          <t>5052</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>L-8 Ingegneria dell'informazione</t>
+          <t>LM-27 Ingegneria delle telecomunicazioni</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Agostino Poggi</t>
+          <t>Alberto Bononi</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1277,22 +1272,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>INGEGNERIA INFORMATICA, ELETTRONICA E DELLE TELECOMUNICAZIONI</t>
+          <t>ELECTRONIC ENGINEERING FOR INTELLIGENT VEHICLES</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3050</t>
+          <t>5076</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>L-8 Ingegneria dell'informazione</t>
+          <t>LM-29 Ingegneria elettronica</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Gianluigi Ferrari</t>
+          <t>Massimo Bertozzi</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1306,22 +1301,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ARCHITETTURA E CITTA’ SOSTENIBILI</t>
+          <t>INGEGNERIA ELETTRONICA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5066</t>
+          <t>5013</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>LM-4 Architettura e ingegneria edile-architettura</t>
+          <t>LM-29 Ingegneria elettronica</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Enrico Prandi</t>
+          <t>Giovanni Chiorboli</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1335,22 +1330,22 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>INGEGNERIA CIVILE</t>
+          <t>INGEGNERIA INFORMATICA</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5011</t>
+          <t>5015</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>LM-23 Ingegneria civile</t>
+          <t>LM-32 Ingegneria informatica</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Francesco Freddi</t>
+          <t>Stefano Cagnoni</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1364,22 +1359,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>COMMUNICATION ENGENEERING</t>
+          <t>INGEGNERIA PER L'AMBIENTE E IL TERRITORIO</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5052</t>
+          <t>5018</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>LM-27 Ingegneria delle telecomunicazioni</t>
+          <t>LM-35 Ingegneria per l'ambiente e il territorio</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Alberto Bononi</t>
+          <t>Riccardo Roncella</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1393,22 +1388,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ELECTRONIC ENGINEERING FOR INTELLIGENT VEHICLES</t>
+          <t>COSTRUZIONI, INFRASTRUTTURE E TERRITORIO</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5076</t>
+          <t>3059</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>LM-29 Ingegneria elettronica</t>
+          <t>L-P01 Professioni Tecniche per l’edilizia e il territorio</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Massimo Bertozzi</t>
+          <t>Andrea Maranzoni</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1422,374 +1417,406 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>INGEGNERIA ELETTRONICA</t>
+          <t>INGEGNERIA GESTIONALE</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5013</t>
+          <t>3010</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LM-29 Ingegneria elettronica</t>
+          <t>L-9 Ingegneria industriale</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Giovanni Chiorboli</t>
+          <t>Barbara Bigliardi</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
+          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>INGEGNERIA INFORMATICA</t>
+          <t>INGEGNERIA MECCANICA</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5015</t>
+          <t>3011</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LM-32 Ingegneria informatica</t>
+          <t>L-9 Ingegneria industriale</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Stefano Cagnoni</t>
+          <t>Fabio Bozzoli</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
+          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ADVANCED AUTOMOTIVE ENGINEERING</t>
+          <t>INGEGNERIA GESTIONALE</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5057</t>
+          <t>5014</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LM-33 Ingegneria meccanica</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>INTERATENEO BOLOGNA, MODENA E REGGIO EMILIA, FERRARA – SEDE AMM.VA MODENA REGGIO EMILIA</t>
-        </is>
-      </c>
+          <t>LM-31 Ingegneria gestionale</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Francesco Zammori</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
+          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>INGEGNERIA PER L'AMBIENTE E IL TERRITORIO</t>
+          <t>INGEGNERIA MECCANICA</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5018</t>
+          <t>5016</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LM-35 Ingegneria per l'ambiente e il territorio</t>
+          <t>LM-33 Ingegneria meccanica</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Riccardo Roncella</t>
+          <t>Luca Collini</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
+          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>COSTRUZIONI, INFRASTRUTTURE E TERRITORIO</t>
+          <t>ENGINEERING FOR THE FOOD INDUSTRY</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3059</t>
+          <t>5075</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>L-P01 Professioni Tecniche per l’edilizia e il territorio</t>
+          <t>LM-33 Ingegneria meccanica</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Andrea Maranzoni</t>
+          <t>Giuseppe Vignali</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
+          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ADVANCED AUTOMOTIVE ELECTRONIC ENGINEERING</t>
+          <t>SCIENZE MOTORIE, SPORT E SALUTE</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5058</t>
+          <t>3019</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LM-29 – Ingegneria Elettronica</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>INTERATENEO – SEDE AMM.VA BOLOGNA</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
+          <t>L-22 Scienze delle attività motorie e sportive</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Giuliana Gobbi</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>5  DI CUI 3 PO/PA</t>
+        </is>
+      </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
+          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ELECTRIC VEHICLE ENGINEERING</t>
+          <t>INFERMIERISTICA</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5070</t>
+          <t>3040</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LM-28 – Ingegneria Elettrica</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>INTERATENEO – SEDE AMM.VA BOLOGNA</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr"/>
+          <t>L/SNT1 Professioni sanitarie, infermieristiche e professione sanitaria ostetrica</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Elena Bignami</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA  DI INGEGNERIA E ARCHITETTURA</t>
+          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>INGEGNERIA GESTIONALE</t>
+          <t>OSTETRICIA</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>3010</t>
+          <t>3041</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>L-9 Ingegneria industriale</t>
+          <t>L/SNT1 Professioni sanitarie, infermieristiche e professione sanitaria ostetrica</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Barbara Bigliardi</t>
+          <t>Tullio Ghi</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
+          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>INGEGNERIA MECCANICA</t>
+          <t>FISIOTERAPIA</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3011</t>
+          <t>3042</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>L-9 Ingegneria industriale</t>
+          <t>L/SNT2 Professioni sanitarie della riabilitazione</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Fabio Bozzoli</t>
+          <t>Cosimo Costantino</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
+          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>INGEGNERIA GESTIONALE</t>
+          <t>LOGOPEDIA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5014</t>
+          <t>3043</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>LM-31 Ingegneria gestionale</t>
+          <t>L/SNT2 Professioni sanitarie della riabilitazione</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Francesco Zammori</t>
+          <t>Andrea Bacciu</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
+          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>INGEGNERIA MECCANICA</t>
+          <t>ORTOTTICA ED ASSISTENZA OFTALMOLOGICA</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5016</t>
+          <t>3044</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>LM-33 Ingegneria meccanica</t>
+          <t>L/SNT2 Professioni sanitarie della riabilitazione</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Luca Collini</t>
+          <t>Paolo Mora</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
+          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ENGINEERING FOR THE FOOD INDUSTRY</t>
+          <t>EDUCAZIONE PROFESSIONALE</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5075</t>
+          <t>3067</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>LM-33 Ingegneria meccanica</t>
+          <t>L/SNT2 Professioni sanitarie della riabilitazione</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Giuseppe Vignali</t>
+          <t>Referente: Carlo Marchesi</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)  DI INGEGNERIA DEI SISTEMI E DELLE TECNOLOGIE INDUSTRIALI (DISTI)</t>
+          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ASSISTENZA SANITARIA</t>
+          <t>TECNICHE AUDIOPROTESICHE</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>3065</t>
+          <t>3046</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>L/SNT4 Professioni sanitarie della prevenzione</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>INTERATENEO CON MODENA, REGGIO EMILIA – SEDE AMM.VA MODENA</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr"/>
+          <t>L/SNT3 Professioni sanitarie tecniche</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Vincenzo Vincenti</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G46" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
@@ -1799,28 +1826,28 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>SCIENZE MOTORIE, SPORT E SALUTE</t>
+          <t>TECNICHE DI LABORATORIO BIOMEDICO</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>3019</t>
+          <t>3047</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>L-22 Scienze delle attività motorie e sportive</t>
+          <t>L/SNT3 Professioni sanitarie tecniche</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Giuliana Gobbi</t>
+          <t>Federica Maria Angela Rizzi</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>5  DI CUI 3 PO/PA</t>
+          <t>4 DI CUI 2 PO/PA</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -1832,26 +1859,30 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>SCIENZE E TECNICHE PSICOLOGICHE</t>
+          <t>TECNICHE DI RADIOLOGIA MEDICA, PER IMMAGINI E RADIOTERAPIA</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>3021</t>
+          <t>3048</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>L-24 Scienze e tecniche psicologiche</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>INTERATENEO CON MODENA – REGGIO EMILIA SEDE AMM.VA MODENA</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr"/>
+          <t>L/SNT3 Professioni sanitarie tecniche</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Mario Silva</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G48" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
@@ -1861,22 +1892,22 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>INFERMIERISTICA</t>
+          <t>DENTAL HYGIENE</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>3040</t>
+          <t>3063</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>L/SNT1 Professioni sanitarie, infermieristiche e professione sanitaria ostetrica</t>
+          <t>L/SNT3 Professioni sanitarie tecniche</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Elena Bignami</t>
+          <t>Referente: Silvia Pizzi</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -1894,22 +1925,22 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>OSTETRICIA</t>
+          <t>TECNICHE DELLA PREVENZIONE NELL'AMBIENTE E NEI LUOGHI DI LAVORO</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>3041</t>
+          <t>3049</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>L/SNT1 Professioni sanitarie, infermieristiche e professione sanitaria ostetrica</t>
+          <t>L/SNT4 Professioni sanitarie della prevenzione</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Tullio Ghi</t>
+          <t>Roberta Andreoli</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -1927,30 +1958,26 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>FISIOTERAPIA</t>
+          <t>BIOTECNOLOGIE MEDICHE, VETERINARIE E FARMACEUTICHE</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>3042</t>
+          <t>5045</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>L/SNT2 Professioni sanitarie della riabilitazione</t>
+          <t>LM-9 Biotecnologie mediche, veterinarie e farmaceutiche</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Cosimo Costantino</t>
+          <t>Nicola Giuliani</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
@@ -1960,30 +1987,26 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>LOGOPEDIA</t>
+          <t>MEDICINA E CHIRURGIA</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>3043</t>
+          <t>5026</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>L/SNT2 Professioni sanitarie della riabilitazione</t>
+          <t>LM-41 Medicina e chirurgia</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Andrea Bacciu</t>
+          <t>Marcello Giuseppe Maggio</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
@@ -1993,30 +2016,26 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ORTOTTICA ED ASSISTENZA OFTALMOLOGICA</t>
+          <t>ODONTOIATRIA E PROTESI DENTARIA</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>3044</t>
+          <t>5027</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>L/SNT2 Professioni sanitarie della riabilitazione</t>
+          <t>LM-46 Odontoiatria e protesi dentaria</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Paolo Mora</t>
+          <t>Maddalena Manfredi</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
@@ -2026,30 +2045,26 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>EDUCAZIONE PROFESSIONALE</t>
+          <t>PSICOBIOLOGIA E NEUROSCIENZE COGNITIVE</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>3067</t>
+          <t>5053</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>L/SNT2 Professioni sanitarie della riabilitazione</t>
+          <t>LM-51 Psicologia</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Referente: Carlo Marchesi</t>
+          <t>Leonardi Fogassi</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
@@ -2059,22 +2074,22 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>TECNICHE AUDIOPROTESICHE</t>
+          <t>SCIENZE E TECNICHE DELLE ATTIVITÀ MOTORIE PREVENTIVE E ADATTATE</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>3046</t>
+          <t>5028</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>L/SNT3 Professioni sanitarie tecniche</t>
+          <t>LM-67 Scienze e tecniche delle attività motorie preventive e adattate</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Vincenzo Vincenti</t>
+          <t>Prisco Mirandola</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -2092,28 +2107,28 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>TECNICHE DI LABORATORIO BIOMEDICO</t>
+          <t>SCIENZE INFERMIERISTICHE E OSTETRICHE</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>3047</t>
+          <t>5050</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>L/SNT3 Professioni sanitarie tecniche</t>
+          <t>LM/SNT1 Scienze infermieristiche e ostetriche</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Federica Maria Angela Rizzi</t>
+          <t>Giuseppe Pedrazzi</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>4 DI CUI 2 PO/PA</t>
+          <t>3 DI CUI 1 PO/PA</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2125,406 +2140,370 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>TECNICHE DI RADIOLOGIA MEDICA, PER IMMAGINI E RADIOTERAPIA</t>
+          <t>BIOTECNOLOGIE</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>3048</t>
+          <t>3022</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>L/SNT3 Professioni sanitarie tecniche</t>
+          <t>L-2 Biotecnologie</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Mario Silva</t>
+          <t>Mariolina Gullì</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>DENTAL HYGIENE</t>
+          <t>BIOLOGIA</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>3063</t>
+          <t>3023</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>L/SNT3 Professioni sanitarie tecniche</t>
+          <t>L-13 Scienze biologiche</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Referente: Silvia Pizzi</t>
+          <t>Valeria Rossi</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>TECNICHE DELLA PREVENZIONE NELL'AMBIENTE E NEI LUOGHI DI LAVORO</t>
+          <t>CHIMICA</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>3049</t>
+          <t>3024</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>L/SNT4 Professioni sanitarie della prevenzione</t>
+          <t>L-27 Scienze e tecnologie chimiche</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Roberta Andreoli</t>
+          <t>Alessia Bacchi</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>BIOTECNOLOGIE MEDICHE, VETERINARIE E FARMACEUTICHE</t>
+          <t>SCIENZE DELLA NATURA E DELL'AMBIENTE</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>5045</t>
+          <t>3028</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>LM-9 Biotecnologie mediche, veterinarie e farmaceutiche</t>
+          <t>L-32 Scienze e tecnologie per l'ambiente e la natura</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Nicola Giuliani</t>
+          <t>Alessandro Petraglia</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MEDICINA E CHIRURGIA</t>
+          <t>SCIENZE GEOLOGICHE</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>5026</t>
+          <t>3029</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>LM-41 Medicina e chirurgia</t>
+          <t>L-34 Scienze geologiche</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Marcello Giuseppe Maggio</t>
+          <t>Alessandro Chelli</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MEDICINE AND SURGERY</t>
+          <t>SCIENZA DEI MATERIALI</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>5074</t>
+          <t>3062</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>LM-41 Medicina e chirurgia</t>
+          <t>L-SC.MAT Scienze dei materiali</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Antonio Percesepe</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>SEDE DI PIACENZA</t>
-        </is>
-      </c>
+          <t>Ludovico Cademartiri</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>ODONTOIATRIA E PROTESI DENTARIA</t>
+          <t>SCIENZE BIOMEDICHE TRASLAZIONALI</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>5027</t>
+          <t>5071</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>LM-46 Odontoiatria e protesi dentaria</t>
+          <t>LM-6 Biologia</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Maddalena Manfredi</t>
+          <t>Annamaria Buschini</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>PSICOBIOLOGIA E NEUROSCIENZE COGNITIVE</t>
+          <t>ECOLOGIA ED ETOLOGIA PER LA CONSERVAZIONE DELLA NATURA</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5053</t>
+          <t>5061</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>LM-51 Psicologia</t>
+          <t>LM-6 Biologia</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Leonardi Fogassi</t>
+          <t>Paola Maria Valsecchi</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>SCIENZE E TECNICHE DELLE ATTIVITÀ MOTORIE PREVENTIVE E ADATTATE</t>
+          <t>SCIENZE BIOMOLECOLARI, GENOMICHE E CELLULARI</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>5028</t>
+          <t>5062</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>LM-67 Scienze e tecniche delle attività motorie preventive e adattate</t>
+          <t>LM-6 Biologia</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Prisco Mirandola</t>
+          <t>Alessio Peracchi</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>SCIENZE INFERMIERISTICHE E OSTETRICHE</t>
+          <t>BIOTECNOLOGIE GENOMICHE, MOLECOLARI E INDUSTRIALI</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>5050</t>
+          <t>5055</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>LM/SNT1 Scienze infermieristiche e ostetriche</t>
+          <t>LM-8 Biotecnologie industriali</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Giuseppe Pedrazzi</t>
+          <t>Barbara Montanini</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>3 DI CUI 1 PO/PA</t>
-        </is>
-      </c>
+      <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SCIENZE E TECNICHE PSICOLOGICHE PER LE SFIDE CONTEMPORANEE</t>
+          <t>CHIMICA</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>3070</t>
+          <t>5039</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>L-24 Scienze e Tecniche Psicologiche</t>
+          <t>LM-54 Scienze chimiche</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Luca Bonini (referente)</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>ATTIVO DALL’A.A. 2024/25</t>
-        </is>
-      </c>
+          <t>Alessia Bacchi</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>TERAPIA DELLA NEURO E PSICOMOTRICITA’ DELL’ETA’ EVOLUTIVA</t>
+          <t>CHIMICA INDUSTRIALE</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>3071</t>
+          <t>5041</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>L-SNT2 Professioni Sanitarie della Riabilitazione</t>
+          <t>M-71 Scienze e tecnologie della chimica industriale</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Stefano Rozzi (referente)</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>ATTIVO DALL’A.A. 2024/25</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>3 DI CUI 1 PO/PA</t>
-        </is>
-      </c>
+          <t>Alessia Bacchi</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA  DI MEDICINA E CHIRURGIA</t>
+          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>BIOTECNOLOGIE</t>
+          <t>SCIENZE GEOLOGICHE APPLICATE ALLA SOSTENIBILITÀ AMBIENTALE</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>3022</t>
+          <t>5072</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>L-2 Biotecnologie</t>
+          <t>LM-74 Scienze e tecnologie geologiche</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Mariolina Gullì</t>
+          <t>Alessandro Chelli</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -2538,22 +2517,22 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>BIOLOGIA</t>
+          <t>SCIENZE E TECNOLOGIE PER L'AMBIENTE E LE RISORSE</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>3023</t>
+          <t>5043</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>L-13 Scienze biologiche</t>
+          <t>LM-75 Scienze e tecnologie per l'ambiente e il territorio</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Valeria Rossi</t>
+          <t>Fulvio Celico</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
@@ -2567,1145 +2546,702 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>CHIMICA</t>
+          <t>QUALITA’ E APPROVVIGIONAMENTO DI MATERIE PRIME PER L’AGRO-ALIMENTARE</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3024</t>
+          <t>3064</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>L-27 Scienze e tecnologie chimiche</t>
+          <t>L-P02 Professioni tecniche agrarie, alimentari e forestali</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Alessia Bacchi</t>
+          <t>Tommaso Ganino</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>SCIENZE DELLA NATURA E DELL'AMBIENTE</t>
+          <t>SCIENZE GASTRONOMICHE</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>3028</t>
+          <t>3069</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>L-32 Scienze e tecnologie per l'ambiente e la natura</t>
+          <t>L-26 Scienze e Tecnologie Alimentari</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Alessandro Petraglia</t>
+          <t>Cristina Mora</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>SCIENZE GEOLOGICHE</t>
+          <t>SCIENZE E TECNOLOGIE ALIMENTARI</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>3029</t>
+          <t>3000</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>L-34 Scienze geologiche</t>
+          <t>L-26 Scienze e tecnologie alimentari</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Alessandro Chelli</t>
+          <t>Monica Gatti</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>SCIENZA DEI MATERIALI</t>
+          <t>CHIMICA E TECNOLOGIA FARMACEUTICHE</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>3062</t>
+          <t>5080</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>L-SC.MAT Scienze dei materiali</t>
+          <t>LM-13. Farmacia e farmacia industriale</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Ludovico Cademartiri</t>
+          <t>Alessio Lodola</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>SCIENZE BIOMEDICHE TRASLAZIONALI</t>
+          <t>FARMACIA</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>5071</t>
+          <t>5079</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LM-6 Biologia</t>
+          <t>LM-13. Farmacia e farmacia industriale</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Annamaria Buschini</t>
+          <t>Massimiliano Tognolini</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ECOLOGIA ED ETOLOGIA PER LA CONSERVAZIONE DELLA NATURA</t>
+          <t>SCIENZE DELLA NUTRIZIONE UMANA</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>5061</t>
+          <t>5068</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>LM-6 Biologia</t>
+          <t>LM-61 Scienze della nutrizione umana</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Paola Maria Valsecchi</t>
+          <t>Francesca Scazzina</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>SCIENZE BIOMOLECOLARI, GENOMICHE E CELLULARI</t>
+          <t>SCIENZE E TECNOLOGIE ALIMENTARI</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>5062</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>LM-6 Biologia</t>
+          <t>LM-70 Scienze e tecnologie alimentari</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Alessio Peracchi</t>
+          <t>Claudia Folli</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>BIOTECNOLOGIE GENOMICHE, MOLECOLARI E INDUSTRIALI</t>
+          <t>ECONOMIA E MANAGEMENT</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>5055</t>
+          <t>3004</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>LM-8 Biotecnologie industriali</t>
+          <t>L-18 Scienze dell'economia e della gestione aziendale</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Barbara Montanini</t>
+          <t>Katia Furlotti</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>CHIMICA</t>
+          <t>ECONOMIA E MANAGEMENT DELLE FILIERE ALIMENTARI SOSTENIBILI</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>5039</t>
+          <t>3072</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>LM-54 Scienze chimiche</t>
+          <t>L-18 Scienze dell'economia e della gestione aziendale</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Alessia Bacchi</t>
+          <t>Lucia Poletti</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>CHIMICA INDUSTRIALE</t>
+          <t>AMMINISTRAZIONE E DIREZIONE AZIENDALE</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>5041</t>
+          <t>5003</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>M-71 Scienze e tecnologie della chimica industriale</t>
+          <t>LM-77 Scienze economico-aziendali</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Alessia Bacchi</t>
+          <t>Veronica Tibiletti</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>SCIENZE GEOLOGICHE APPLICATE ALLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>FINANZA E RISK MANAGEMENT</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>5072</t>
+          <t>5005</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>LM-74 Scienze e tecnologie geologiche</t>
+          <t>LM-77 Scienze economico-aziendali</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Alessandro Chelli</t>
+          <t>Maria Gaia Soana</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>SCIENZE E TECNOLOGIE PER L'AMBIENTE E LE RISORSE</t>
+          <t>ECONOMIA INTERNAZIONALE E DELLO SVILUPPO - INTERNATIONAL BUSINESS AND DEVELOPMENT</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>5043</t>
+          <t>5047</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>LM-75 Scienze e tecnologie per l'ambiente e il territorio</t>
+          <t>LM-77 Scienze economico-aziendali</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Fulvio Celico</t>
+          <t>Paolo Fabbri</t>
         </is>
       </c>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>FUNCTIONAL AND SUSTAINABLE MATERIALS</t>
+          <t>TRADE E CONSUMER MARKETING</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>5082</t>
+          <t>5059</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>LM Sc. Mat Scienza dei Materiali</t>
+          <t>LM-77 Scienze economico-aziendali</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Anna Painelli (referente)</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>ATTIVO DALL’A.A. 2024/25</t>
-        </is>
-      </c>
+          <t>Cristina Ziliani</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE  DI SCIENZE CHIMICHE, DELLA VITA E DELLA SOSTENIBILITÀ AMBIENTALE</t>
+          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>QUALITA’ E APPROVVIGIONAMENTO DI MATERIE PRIME PER L’AGRO-ALIMENTARE</t>
+          <t>ECONOMIA E MANAGEMENT DEI SISTEMI ALIMENTARI SOSTENIBILI</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>3064</t>
+          <t>5077</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>L-P02 Professioni tecniche agrarie, alimentari e forestali</t>
+          <t>LM-77 Scienze economico-aziendali</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Tommaso Ganino</t>
+          <t>Filippo Arfini</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
+      <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>SCIENZE GASTRONOMICHE</t>
+          <t>FISICA</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>3069</t>
+          <t>3026</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>L-26 Scienze e Tecnologie Alimentari</t>
+          <t>L-30 Scienze e tecnologie fisiche</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Cristina Mora</t>
+          <t>Luigi Cristofolini</t>
         </is>
       </c>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>SCIENZE E TECNOLOGIE ALIMENTARI</t>
+          <t>INFORMATICA</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>3027</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>L-26 Scienze e tecnologie alimentari</t>
+          <t>L-31 Scienze e tecnologie informatiche</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Monica Gatti</t>
+          <t>Alessandro Dal Palù</t>
         </is>
       </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>CHIMICA E TECNOLOGIA FARMACEUTICHE</t>
+          <t>MATEMATICA</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>5080</t>
+          <t>3030</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>LM-13. Farmacia e farmacia industriale</t>
+          <t>L-35 Scienze matematiche</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Alessio Lodola</t>
+          <t>Luca Lorenzi</t>
         </is>
       </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>FARMACIA</t>
+          <t>FISICA</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>5079</t>
+          <t>5036</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>LM-13. Farmacia e farmacia industriale</t>
+          <t>LM-17 Fisica</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Massimiliano Tognolini</t>
+          <t>Luigi Cristofolini</t>
         </is>
       </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>SCIENZE DELLA NUTRIZIONE UMANA</t>
+          <t>SCIENZE INFORMATICHE</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>5068</t>
+          <t>5069</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>LM-61 Scienze della nutrizione umana</t>
+          <t>LM-18 Informatica</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Francesca Scazzina</t>
+          <t>Alessandro Dal Palù</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>SCIENZE E TECNOLOGIE ALIMENTARI</t>
+          <t>MATEMATICA</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>5037</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>LM-70 Scienze e tecnologie alimentari</t>
+          <t>LM-40 Matematica</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Claudia Folli</t>
+          <t>Luca Lorenzi</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>FOOD SAFETY AND FOOD RISK MANAGEMENT</t>
+          <t>SCIENZE ZOOTECNICHE E TECNOLOGIE DELLE PRODUZIONI ANIMALI</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>5064</t>
+          <t>3020</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>LM-70 Scienze e tecnologie alimentari</t>
+          <t>L-38 Scienze zootecniche e tecnologie delle produzioni animali</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Tullia Tedeschi</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>INTERATENEO BOLOGNA, FERRARA, MODENA E REGGIO EMILIA, CATTOLICA DI MILANO (SEDE DI PIACENZA) – SEDE AMM.VA PARMA</t>
-        </is>
-      </c>
+          <t>Claudio Cipolat Gotet</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>FOOD SCIENCES FOR INNOVATION AND AUTHENTICITY</t>
+          <t>MEDICINA VETERINARIA</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>5063</t>
+          <t>5029</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>LM-70 Scienze e tecnologie alimentari</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>INTERATENEO UDINE, BOLZANO – SEDE AMM.VA BOLZANO</t>
-        </is>
-      </c>
+          <t>LM-42 Medicina veterinaria</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Roberta Saleri</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO  DI SCIENZE DEGLI ALIMENTI E DEL FARMACO</t>
+          <t>DIPARTIMENTODI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ECONOMIA E MANAGEMENT</t>
+          <t>PRODUZIONI ANIMALI INNOVATIVE E SOSTENIBILI</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>3004</t>
+          <t>5065</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>L-18 Scienze dell'economia e della gestione aziendale</t>
+          <t>LM-86 Scienze zootecniche e tecnologie animali</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Katia Furlotti</t>
+          <t>Massimo Malacarne</t>
         </is>
       </c>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr">
         <is>
-          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
+          <t>DIPARTIMENTODI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ECONOMIA E MANAGEMENT DELLE FILIERE ALIMENTARI SOSTENIBILI</t>
+          <t>TECNOLOGIE E GESTIONE DELL’IMPRESA CASEARIA</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>3072</t>
+          <t>3068</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>L-18 Scienze dell'economia e della gestione aziendale</t>
+          <t>L-P02 Professioni tecniche agrarie, alimentari e forestali</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Lucia Poletti</t>
+          <t>Andrea Summer</t>
         </is>
       </c>
       <c r="E94" t="inlineStr"/>
-      <c r="F94" t="inlineStr"/>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>4 DI CUI 2 PO/PA</t>
+        </is>
+      </c>
       <c r="G94" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>AMMINISTRAZIONE E DIREZIONE AZIENDALE</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>5003</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>LM-77 Scienze economico-aziendali</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Veronica Tibiletti</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>FINANZA E RISK MANAGEMENT</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>5005</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>LM-77 Scienze economico-aziendali</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Maria Gaia Soana</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr"/>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>ECONOMIA INTERNAZIONALE E DELLO SVILUPPO - INTERNATIONAL BUSINESS AND DEVELOPMENT</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>5047</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>LM-77 Scienze economico-aziendali</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>Paolo Fabbri</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr"/>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>TRADE E CONSUMER MARKETING</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>5059</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>LM-77 Scienze economico-aziendali</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>Cristina Ziliani</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>ECONOMIA E MANAGEMENT DEI SISTEMI ALIMENTARI SOSTENIBILI</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>5077</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>LM-77 Scienze economico-aziendali</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>Filippo Arfini</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI  DI SCIENZE ECONOMICHE E AZIENDALI</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>FISICA</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>3026</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>L-30 Scienze e tecnologie fisiche</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>Luigi Cristofolini</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr"/>
-      <c r="F100" t="inlineStr"/>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>INFORMATICA</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>3027</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>L-31 Scienze e tecnologie informatiche</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Alessandro Dal Palù</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr"/>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>MATEMATICA</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>3030</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>L-35 Scienze matematiche</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Luca Lorenzi</t>
-        </is>
-      </c>
-      <c r="E102" t="inlineStr"/>
-      <c r="F102" t="inlineStr"/>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>FISICA</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>5036</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>LM-17 Fisica</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Luigi Cristofolini</t>
-        </is>
-      </c>
-      <c r="E103" t="inlineStr"/>
-      <c r="F103" t="inlineStr"/>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>SCIENZE INFORMATICHE</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>5069</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>LM-18 Informatica</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Alessandro Dal Palù</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr"/>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>MATEMATICA</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>5037</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>LM-40 Matematica</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Luca Lorenzi</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr"/>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE  DI SCIENZE MATEMATICHE, FISICHE E INFORMATICHE</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>SCIENZE ZOOTECNICHE E TECNOLOGIE DELLE PRODUZIONI ANIMALI</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>3020</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>L-38 Scienze zootecniche e tecnologie delle produzioni animali</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Claudio Cipolat Gotet</t>
-        </is>
-      </c>
-      <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>MEDICINA VETERINARIA</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>5029</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>LM-42 Medicina veterinaria</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Roberta Saleri</t>
-        </is>
-      </c>
-      <c r="E107" t="inlineStr"/>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>PRODUZIONI ANIMALI INNOVATIVE E SOSTENIBILI</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>5065</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>LM-86 Scienze zootecniche e tecnologie animali</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Massimo Malacarne</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr"/>
-      <c r="F108" t="inlineStr"/>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>DIPARTIMENTODI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>TECNOLOGIE E GESTIONE DELL’IMPRESA CASEARIA</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>3068</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>L-P02 Professioni tecniche agrarie, alimentari e forestali</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Andrea Summer</t>
-        </is>
-      </c>
-      <c r="E109" t="inlineStr"/>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>4 DI CUI 2 PO/PA</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
         <is>
           <t>DIPARTIMENTODI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE  DI SCIENZE MEDICO-VETERINARIE</t>
         </is>

</xml_diff>